<commit_message>
Back to the original error after changing all of this stuff!
Error is if (sex == 0) { : missing value where TRUE/FALSE needed
</commit_message>
<xml_diff>
--- a/data/hake_from_ss.xlsx
+++ b/data/hake_from_ss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D996BD36-13F6-264C-A00C-2F1BBE80AAAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBF6D64-B2BE-A945-89B3-708FE4630ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30080" yWindow="500" windowWidth="30080" windowHeight="33340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="494">
   <si>
     <t>Number</t>
   </si>
@@ -1242,6 +1242,297 @@
   </si>
   <si>
     <t>Hake_wt</t>
+  </si>
+  <si>
+    <t>Length_21</t>
+  </si>
+  <si>
+    <t>Length_22</t>
+  </si>
+  <si>
+    <t>Length_23</t>
+  </si>
+  <si>
+    <t>Length_24</t>
+  </si>
+  <si>
+    <t>Length_25</t>
+  </si>
+  <si>
+    <t>Length_26</t>
+  </si>
+  <si>
+    <t>Length_27</t>
+  </si>
+  <si>
+    <t>Length_28</t>
+  </si>
+  <si>
+    <t>Length_29</t>
+  </si>
+  <si>
+    <t>Length_30</t>
+  </si>
+  <si>
+    <t>Length_31</t>
+  </si>
+  <si>
+    <t>Length_32</t>
+  </si>
+  <si>
+    <t>Length_33</t>
+  </si>
+  <si>
+    <t>Length_34</t>
+  </si>
+  <si>
+    <t>Length_35</t>
+  </si>
+  <si>
+    <t>Length_36</t>
+  </si>
+  <si>
+    <t>Length_37</t>
+  </si>
+  <si>
+    <t>Length_38</t>
+  </si>
+  <si>
+    <t>Length_39</t>
+  </si>
+  <si>
+    <t>Length_40</t>
+  </si>
+  <si>
+    <t>Length_41</t>
+  </si>
+  <si>
+    <t>Length_42</t>
+  </si>
+  <si>
+    <t>Length_43</t>
+  </si>
+  <si>
+    <t>Length_44</t>
+  </si>
+  <si>
+    <t>Length_45</t>
+  </si>
+  <si>
+    <t>Length_46</t>
+  </si>
+  <si>
+    <t>Length_47</t>
+  </si>
+  <si>
+    <t>Length_48</t>
+  </si>
+  <si>
+    <t>Length_49</t>
+  </si>
+  <si>
+    <t>Length_50</t>
+  </si>
+  <si>
+    <t>Length_51</t>
+  </si>
+  <si>
+    <t>Length_52</t>
+  </si>
+  <si>
+    <t>Length_53</t>
+  </si>
+  <si>
+    <t>Length_54</t>
+  </si>
+  <si>
+    <t>Length_55</t>
+  </si>
+  <si>
+    <t>Length_56</t>
+  </si>
+  <si>
+    <t>Length_57</t>
+  </si>
+  <si>
+    <t>Length_58</t>
+  </si>
+  <si>
+    <t>Length_59</t>
+  </si>
+  <si>
+    <t>Length_60</t>
+  </si>
+  <si>
+    <t>Length_61</t>
+  </si>
+  <si>
+    <t>Length_62</t>
+  </si>
+  <si>
+    <t>Length_63</t>
+  </si>
+  <si>
+    <t>Length_64</t>
+  </si>
+  <si>
+    <t>Length_65</t>
+  </si>
+  <si>
+    <t>Length_66</t>
+  </si>
+  <si>
+    <t>Length_67</t>
+  </si>
+  <si>
+    <t>Length_68</t>
+  </si>
+  <si>
+    <t>Length_69</t>
+  </si>
+  <si>
+    <t>Length_70</t>
+  </si>
+  <si>
+    <t>Length_71</t>
+  </si>
+  <si>
+    <t>Length_72</t>
+  </si>
+  <si>
+    <t>Length_73</t>
+  </si>
+  <si>
+    <t>Length_74</t>
+  </si>
+  <si>
+    <t>Length_75</t>
+  </si>
+  <si>
+    <t>Length_76</t>
+  </si>
+  <si>
+    <t>Length_77</t>
+  </si>
+  <si>
+    <t>Length_78</t>
+  </si>
+  <si>
+    <t>Length_79</t>
+  </si>
+  <si>
+    <t>Length_80</t>
+  </si>
+  <si>
+    <t>Length_81</t>
+  </si>
+  <si>
+    <t>Length_82</t>
+  </si>
+  <si>
+    <t>Length_83</t>
+  </si>
+  <si>
+    <t>Length_84</t>
+  </si>
+  <si>
+    <t>Length_85</t>
+  </si>
+  <si>
+    <t>Length_86</t>
+  </si>
+  <si>
+    <t>Length_87</t>
+  </si>
+  <si>
+    <t>Length_88</t>
+  </si>
+  <si>
+    <t>Length_89</t>
+  </si>
+  <si>
+    <t>Length_90</t>
+  </si>
+  <si>
+    <t>Length_91</t>
+  </si>
+  <si>
+    <t>Length_92</t>
+  </si>
+  <si>
+    <t>Length_93</t>
+  </si>
+  <si>
+    <t>Length_94</t>
+  </si>
+  <si>
+    <t>Length_95</t>
+  </si>
+  <si>
+    <t>Length_96</t>
+  </si>
+  <si>
+    <t>Length_97</t>
+  </si>
+  <si>
+    <t>Length_98</t>
+  </si>
+  <si>
+    <t>Length_99</t>
+  </si>
+  <si>
+    <t>Length_100</t>
+  </si>
+  <si>
+    <t>Length_101</t>
+  </si>
+  <si>
+    <t>Length_102</t>
+  </si>
+  <si>
+    <t>Length_103</t>
+  </si>
+  <si>
+    <t>Length_104</t>
+  </si>
+  <si>
+    <t>Length_105</t>
+  </si>
+  <si>
+    <t>Length_106</t>
+  </si>
+  <si>
+    <t>Length_107</t>
+  </si>
+  <si>
+    <t>Length_108</t>
+  </si>
+  <si>
+    <t>Length_109</t>
+  </si>
+  <si>
+    <t>Length_110</t>
+  </si>
+  <si>
+    <t>Length_111</t>
+  </si>
+  <si>
+    <t>Length_112</t>
+  </si>
+  <si>
+    <t>Length_113</t>
+  </si>
+  <si>
+    <t>Length_114</t>
+  </si>
+  <si>
+    <t>Length_115</t>
+  </si>
+  <si>
+    <t>Length_116</t>
+  </si>
+  <si>
+    <t>Length_117</t>
   </si>
 </sst>
 </file>
@@ -9378,7 +9669,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9477,7 +9768,7 @@
         <v>49</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -9646,7 +9937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
@@ -11769,7 +12060,7 @@
   <dimension ref="A1:DU59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E59"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16281,8 +16572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Y109"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="X12" sqref="X12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28820,15 +29111,24 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:DR21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="104" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="105" max="122" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:122" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>325</v>
       </c>
@@ -28904,8 +29204,299 @@
       <c r="Y1" s="1" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z1" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="CV1" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="CW1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="CX1" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="CY1" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="DC1" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="DD1" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="DE1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="DH1" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="DM1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="DN1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="DO1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="DP1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="DR1" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="2" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>395</v>
       </c>
@@ -28981,8 +29572,299 @@
       <c r="Y2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="BD2">
+        <v>0</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BF2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
+      <c r="BH2">
+        <v>0</v>
+      </c>
+      <c r="BI2">
+        <v>0</v>
+      </c>
+      <c r="BJ2">
+        <v>0</v>
+      </c>
+      <c r="BK2">
+        <v>0</v>
+      </c>
+      <c r="BL2">
+        <v>0</v>
+      </c>
+      <c r="BM2">
+        <v>0</v>
+      </c>
+      <c r="BN2">
+        <v>0</v>
+      </c>
+      <c r="BO2">
+        <v>0</v>
+      </c>
+      <c r="BP2">
+        <v>0</v>
+      </c>
+      <c r="BQ2">
+        <v>0</v>
+      </c>
+      <c r="BR2">
+        <v>0</v>
+      </c>
+      <c r="BS2">
+        <v>0</v>
+      </c>
+      <c r="BT2">
+        <v>0</v>
+      </c>
+      <c r="BU2">
+        <v>0</v>
+      </c>
+      <c r="BV2">
+        <v>0</v>
+      </c>
+      <c r="BW2">
+        <v>0</v>
+      </c>
+      <c r="BX2">
+        <v>0</v>
+      </c>
+      <c r="BY2">
+        <v>0</v>
+      </c>
+      <c r="BZ2">
+        <v>0</v>
+      </c>
+      <c r="CA2">
+        <v>0</v>
+      </c>
+      <c r="CB2">
+        <v>0</v>
+      </c>
+      <c r="CC2">
+        <v>0</v>
+      </c>
+      <c r="CD2">
+        <v>0</v>
+      </c>
+      <c r="CE2">
+        <v>0</v>
+      </c>
+      <c r="CF2">
+        <v>0</v>
+      </c>
+      <c r="CG2">
+        <v>0</v>
+      </c>
+      <c r="CH2">
+        <v>0</v>
+      </c>
+      <c r="CI2">
+        <v>0</v>
+      </c>
+      <c r="CJ2">
+        <v>0</v>
+      </c>
+      <c r="CK2">
+        <v>0</v>
+      </c>
+      <c r="CL2">
+        <v>0</v>
+      </c>
+      <c r="CM2">
+        <v>0</v>
+      </c>
+      <c r="CN2">
+        <v>0</v>
+      </c>
+      <c r="CO2">
+        <v>0</v>
+      </c>
+      <c r="CP2">
+        <v>0</v>
+      </c>
+      <c r="CQ2">
+        <v>0</v>
+      </c>
+      <c r="CR2">
+        <v>0</v>
+      </c>
+      <c r="CS2">
+        <v>0</v>
+      </c>
+      <c r="CT2">
+        <v>0</v>
+      </c>
+      <c r="CU2">
+        <v>0</v>
+      </c>
+      <c r="CV2">
+        <v>0</v>
+      </c>
+      <c r="CW2">
+        <v>0</v>
+      </c>
+      <c r="CX2">
+        <v>0</v>
+      </c>
+      <c r="CY2">
+        <v>0</v>
+      </c>
+      <c r="CZ2">
+        <v>0</v>
+      </c>
+      <c r="DA2">
+        <v>0</v>
+      </c>
+      <c r="DB2">
+        <v>0</v>
+      </c>
+      <c r="DC2">
+        <v>0</v>
+      </c>
+      <c r="DD2">
+        <v>0</v>
+      </c>
+      <c r="DE2">
+        <v>0</v>
+      </c>
+      <c r="DF2">
+        <v>0</v>
+      </c>
+      <c r="DG2">
+        <v>0</v>
+      </c>
+      <c r="DH2">
+        <v>0</v>
+      </c>
+      <c r="DI2">
+        <v>0</v>
+      </c>
+      <c r="DJ2">
+        <v>0</v>
+      </c>
+      <c r="DK2">
+        <v>0</v>
+      </c>
+      <c r="DL2">
+        <v>0</v>
+      </c>
+      <c r="DM2">
+        <v>0</v>
+      </c>
+      <c r="DN2">
+        <v>0</v>
+      </c>
+      <c r="DO2">
+        <v>0</v>
+      </c>
+      <c r="DP2">
+        <v>0</v>
+      </c>
+      <c r="DQ2">
+        <v>0</v>
+      </c>
+      <c r="DR2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>395</v>
       </c>
@@ -29058,8 +29940,299 @@
       <c r="Y3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
+      </c>
+      <c r="AZ3">
+        <v>0</v>
+      </c>
+      <c r="BA3">
+        <v>0</v>
+      </c>
+      <c r="BB3">
+        <v>0</v>
+      </c>
+      <c r="BC3">
+        <v>0</v>
+      </c>
+      <c r="BD3">
+        <v>0</v>
+      </c>
+      <c r="BE3">
+        <v>0</v>
+      </c>
+      <c r="BF3">
+        <v>0</v>
+      </c>
+      <c r="BG3">
+        <v>0</v>
+      </c>
+      <c r="BH3">
+        <v>0</v>
+      </c>
+      <c r="BI3">
+        <v>0</v>
+      </c>
+      <c r="BJ3">
+        <v>0</v>
+      </c>
+      <c r="BK3">
+        <v>0</v>
+      </c>
+      <c r="BL3">
+        <v>0</v>
+      </c>
+      <c r="BM3">
+        <v>0</v>
+      </c>
+      <c r="BN3">
+        <v>0</v>
+      </c>
+      <c r="BO3">
+        <v>0</v>
+      </c>
+      <c r="BP3">
+        <v>0</v>
+      </c>
+      <c r="BQ3">
+        <v>0</v>
+      </c>
+      <c r="BR3">
+        <v>0</v>
+      </c>
+      <c r="BS3">
+        <v>0</v>
+      </c>
+      <c r="BT3">
+        <v>0</v>
+      </c>
+      <c r="BU3">
+        <v>0</v>
+      </c>
+      <c r="BV3">
+        <v>0</v>
+      </c>
+      <c r="BW3">
+        <v>0</v>
+      </c>
+      <c r="BX3">
+        <v>0</v>
+      </c>
+      <c r="BY3">
+        <v>0</v>
+      </c>
+      <c r="BZ3">
+        <v>0</v>
+      </c>
+      <c r="CA3">
+        <v>0</v>
+      </c>
+      <c r="CB3">
+        <v>0</v>
+      </c>
+      <c r="CC3">
+        <v>0</v>
+      </c>
+      <c r="CD3">
+        <v>0</v>
+      </c>
+      <c r="CE3">
+        <v>0</v>
+      </c>
+      <c r="CF3">
+        <v>0</v>
+      </c>
+      <c r="CG3">
+        <v>0</v>
+      </c>
+      <c r="CH3">
+        <v>0</v>
+      </c>
+      <c r="CI3">
+        <v>0</v>
+      </c>
+      <c r="CJ3">
+        <v>0</v>
+      </c>
+      <c r="CK3">
+        <v>0</v>
+      </c>
+      <c r="CL3">
+        <v>0</v>
+      </c>
+      <c r="CM3">
+        <v>0</v>
+      </c>
+      <c r="CN3">
+        <v>0</v>
+      </c>
+      <c r="CO3">
+        <v>0</v>
+      </c>
+      <c r="CP3">
+        <v>0</v>
+      </c>
+      <c r="CQ3">
+        <v>0</v>
+      </c>
+      <c r="CR3">
+        <v>0</v>
+      </c>
+      <c r="CS3">
+        <v>0</v>
+      </c>
+      <c r="CT3">
+        <v>0</v>
+      </c>
+      <c r="CU3">
+        <v>0</v>
+      </c>
+      <c r="CV3">
+        <v>0</v>
+      </c>
+      <c r="CW3">
+        <v>0</v>
+      </c>
+      <c r="CX3">
+        <v>0</v>
+      </c>
+      <c r="CY3">
+        <v>0</v>
+      </c>
+      <c r="CZ3">
+        <v>0</v>
+      </c>
+      <c r="DA3">
+        <v>0</v>
+      </c>
+      <c r="DB3">
+        <v>0</v>
+      </c>
+      <c r="DC3">
+        <v>0</v>
+      </c>
+      <c r="DD3">
+        <v>0</v>
+      </c>
+      <c r="DE3">
+        <v>0</v>
+      </c>
+      <c r="DF3">
+        <v>0</v>
+      </c>
+      <c r="DG3">
+        <v>0</v>
+      </c>
+      <c r="DH3">
+        <v>0</v>
+      </c>
+      <c r="DI3">
+        <v>0</v>
+      </c>
+      <c r="DJ3">
+        <v>0</v>
+      </c>
+      <c r="DK3">
+        <v>0</v>
+      </c>
+      <c r="DL3">
+        <v>0</v>
+      </c>
+      <c r="DM3">
+        <v>0</v>
+      </c>
+      <c r="DN3">
+        <v>0</v>
+      </c>
+      <c r="DO3">
+        <v>0</v>
+      </c>
+      <c r="DP3">
+        <v>0</v>
+      </c>
+      <c r="DQ3">
+        <v>0</v>
+      </c>
+      <c r="DR3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>395</v>
       </c>
@@ -29135,8 +30308,299 @@
       <c r="Y4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>0</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="AZ4">
+        <v>0</v>
+      </c>
+      <c r="BA4">
+        <v>0</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
+      <c r="BC4">
+        <v>0</v>
+      </c>
+      <c r="BD4">
+        <v>0</v>
+      </c>
+      <c r="BE4">
+        <v>0</v>
+      </c>
+      <c r="BF4">
+        <v>0</v>
+      </c>
+      <c r="BG4">
+        <v>0</v>
+      </c>
+      <c r="BH4">
+        <v>0</v>
+      </c>
+      <c r="BI4">
+        <v>0</v>
+      </c>
+      <c r="BJ4">
+        <v>0</v>
+      </c>
+      <c r="BK4">
+        <v>0</v>
+      </c>
+      <c r="BL4">
+        <v>0</v>
+      </c>
+      <c r="BM4">
+        <v>0</v>
+      </c>
+      <c r="BN4">
+        <v>0</v>
+      </c>
+      <c r="BO4">
+        <v>0</v>
+      </c>
+      <c r="BP4">
+        <v>0</v>
+      </c>
+      <c r="BQ4">
+        <v>0</v>
+      </c>
+      <c r="BR4">
+        <v>0</v>
+      </c>
+      <c r="BS4">
+        <v>0</v>
+      </c>
+      <c r="BT4">
+        <v>0</v>
+      </c>
+      <c r="BU4">
+        <v>0</v>
+      </c>
+      <c r="BV4">
+        <v>0</v>
+      </c>
+      <c r="BW4">
+        <v>0</v>
+      </c>
+      <c r="BX4">
+        <v>0</v>
+      </c>
+      <c r="BY4">
+        <v>0</v>
+      </c>
+      <c r="BZ4">
+        <v>0</v>
+      </c>
+      <c r="CA4">
+        <v>0</v>
+      </c>
+      <c r="CB4">
+        <v>0</v>
+      </c>
+      <c r="CC4">
+        <v>0</v>
+      </c>
+      <c r="CD4">
+        <v>0</v>
+      </c>
+      <c r="CE4">
+        <v>0</v>
+      </c>
+      <c r="CF4">
+        <v>0</v>
+      </c>
+      <c r="CG4">
+        <v>0</v>
+      </c>
+      <c r="CH4">
+        <v>0</v>
+      </c>
+      <c r="CI4">
+        <v>0</v>
+      </c>
+      <c r="CJ4">
+        <v>0</v>
+      </c>
+      <c r="CK4">
+        <v>0</v>
+      </c>
+      <c r="CL4">
+        <v>0</v>
+      </c>
+      <c r="CM4">
+        <v>0</v>
+      </c>
+      <c r="CN4">
+        <v>0</v>
+      </c>
+      <c r="CO4">
+        <v>0</v>
+      </c>
+      <c r="CP4">
+        <v>0</v>
+      </c>
+      <c r="CQ4">
+        <v>0</v>
+      </c>
+      <c r="CR4">
+        <v>0</v>
+      </c>
+      <c r="CS4">
+        <v>0</v>
+      </c>
+      <c r="CT4">
+        <v>0</v>
+      </c>
+      <c r="CU4">
+        <v>0</v>
+      </c>
+      <c r="CV4">
+        <v>0</v>
+      </c>
+      <c r="CW4">
+        <v>0</v>
+      </c>
+      <c r="CX4">
+        <v>0</v>
+      </c>
+      <c r="CY4">
+        <v>0</v>
+      </c>
+      <c r="CZ4">
+        <v>0</v>
+      </c>
+      <c r="DA4">
+        <v>0</v>
+      </c>
+      <c r="DB4">
+        <v>0</v>
+      </c>
+      <c r="DC4">
+        <v>0</v>
+      </c>
+      <c r="DD4">
+        <v>0</v>
+      </c>
+      <c r="DE4">
+        <v>0</v>
+      </c>
+      <c r="DF4">
+        <v>0</v>
+      </c>
+      <c r="DG4">
+        <v>0</v>
+      </c>
+      <c r="DH4">
+        <v>0</v>
+      </c>
+      <c r="DI4">
+        <v>0</v>
+      </c>
+      <c r="DJ4">
+        <v>0</v>
+      </c>
+      <c r="DK4">
+        <v>0</v>
+      </c>
+      <c r="DL4">
+        <v>0</v>
+      </c>
+      <c r="DM4">
+        <v>0</v>
+      </c>
+      <c r="DN4">
+        <v>0</v>
+      </c>
+      <c r="DO4">
+        <v>0</v>
+      </c>
+      <c r="DP4">
+        <v>0</v>
+      </c>
+      <c r="DQ4">
+        <v>0</v>
+      </c>
+      <c r="DR4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>395</v>
       </c>
@@ -29212,8 +30676,299 @@
       <c r="Y5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
+      </c>
+      <c r="AX5">
+        <v>0</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="AZ5">
+        <v>0</v>
+      </c>
+      <c r="BA5">
+        <v>0</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
+      <c r="BC5">
+        <v>0</v>
+      </c>
+      <c r="BD5">
+        <v>0</v>
+      </c>
+      <c r="BE5">
+        <v>0</v>
+      </c>
+      <c r="BF5">
+        <v>0</v>
+      </c>
+      <c r="BG5">
+        <v>0</v>
+      </c>
+      <c r="BH5">
+        <v>0</v>
+      </c>
+      <c r="BI5">
+        <v>0</v>
+      </c>
+      <c r="BJ5">
+        <v>0</v>
+      </c>
+      <c r="BK5">
+        <v>0</v>
+      </c>
+      <c r="BL5">
+        <v>0</v>
+      </c>
+      <c r="BM5">
+        <v>0</v>
+      </c>
+      <c r="BN5">
+        <v>0</v>
+      </c>
+      <c r="BO5">
+        <v>0</v>
+      </c>
+      <c r="BP5">
+        <v>0</v>
+      </c>
+      <c r="BQ5">
+        <v>0</v>
+      </c>
+      <c r="BR5">
+        <v>0</v>
+      </c>
+      <c r="BS5">
+        <v>0</v>
+      </c>
+      <c r="BT5">
+        <v>0</v>
+      </c>
+      <c r="BU5">
+        <v>0</v>
+      </c>
+      <c r="BV5">
+        <v>0</v>
+      </c>
+      <c r="BW5">
+        <v>0</v>
+      </c>
+      <c r="BX5">
+        <v>0</v>
+      </c>
+      <c r="BY5">
+        <v>0</v>
+      </c>
+      <c r="BZ5">
+        <v>0</v>
+      </c>
+      <c r="CA5">
+        <v>0</v>
+      </c>
+      <c r="CB5">
+        <v>0</v>
+      </c>
+      <c r="CC5">
+        <v>0</v>
+      </c>
+      <c r="CD5">
+        <v>0</v>
+      </c>
+      <c r="CE5">
+        <v>0</v>
+      </c>
+      <c r="CF5">
+        <v>0</v>
+      </c>
+      <c r="CG5">
+        <v>0</v>
+      </c>
+      <c r="CH5">
+        <v>0</v>
+      </c>
+      <c r="CI5">
+        <v>0</v>
+      </c>
+      <c r="CJ5">
+        <v>0</v>
+      </c>
+      <c r="CK5">
+        <v>0</v>
+      </c>
+      <c r="CL5">
+        <v>0</v>
+      </c>
+      <c r="CM5">
+        <v>0</v>
+      </c>
+      <c r="CN5">
+        <v>0</v>
+      </c>
+      <c r="CO5">
+        <v>0</v>
+      </c>
+      <c r="CP5">
+        <v>0</v>
+      </c>
+      <c r="CQ5">
+        <v>0</v>
+      </c>
+      <c r="CR5">
+        <v>0</v>
+      </c>
+      <c r="CS5">
+        <v>0</v>
+      </c>
+      <c r="CT5">
+        <v>0</v>
+      </c>
+      <c r="CU5">
+        <v>0</v>
+      </c>
+      <c r="CV5">
+        <v>0</v>
+      </c>
+      <c r="CW5">
+        <v>0</v>
+      </c>
+      <c r="CX5">
+        <v>0</v>
+      </c>
+      <c r="CY5">
+        <v>0</v>
+      </c>
+      <c r="CZ5">
+        <v>0</v>
+      </c>
+      <c r="DA5">
+        <v>0</v>
+      </c>
+      <c r="DB5">
+        <v>0</v>
+      </c>
+      <c r="DC5">
+        <v>0</v>
+      </c>
+      <c r="DD5">
+        <v>0</v>
+      </c>
+      <c r="DE5">
+        <v>0</v>
+      </c>
+      <c r="DF5">
+        <v>0</v>
+      </c>
+      <c r="DG5">
+        <v>0</v>
+      </c>
+      <c r="DH5">
+        <v>0</v>
+      </c>
+      <c r="DI5">
+        <v>0</v>
+      </c>
+      <c r="DJ5">
+        <v>0</v>
+      </c>
+      <c r="DK5">
+        <v>0</v>
+      </c>
+      <c r="DL5">
+        <v>0</v>
+      </c>
+      <c r="DM5">
+        <v>0</v>
+      </c>
+      <c r="DN5">
+        <v>0</v>
+      </c>
+      <c r="DO5">
+        <v>0</v>
+      </c>
+      <c r="DP5">
+        <v>0</v>
+      </c>
+      <c r="DQ5">
+        <v>0</v>
+      </c>
+      <c r="DR5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>395</v>
       </c>
@@ -29289,8 +31044,299 @@
       <c r="Y6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6">
+        <v>0</v>
+      </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+      <c r="AY6">
+        <v>0</v>
+      </c>
+      <c r="AZ6">
+        <v>0</v>
+      </c>
+      <c r="BA6">
+        <v>0</v>
+      </c>
+      <c r="BB6">
+        <v>0</v>
+      </c>
+      <c r="BC6">
+        <v>0</v>
+      </c>
+      <c r="BD6">
+        <v>0</v>
+      </c>
+      <c r="BE6">
+        <v>0</v>
+      </c>
+      <c r="BF6">
+        <v>0</v>
+      </c>
+      <c r="BG6">
+        <v>0</v>
+      </c>
+      <c r="BH6">
+        <v>0</v>
+      </c>
+      <c r="BI6">
+        <v>0</v>
+      </c>
+      <c r="BJ6">
+        <v>0</v>
+      </c>
+      <c r="BK6">
+        <v>0</v>
+      </c>
+      <c r="BL6">
+        <v>0</v>
+      </c>
+      <c r="BM6">
+        <v>0</v>
+      </c>
+      <c r="BN6">
+        <v>0</v>
+      </c>
+      <c r="BO6">
+        <v>0</v>
+      </c>
+      <c r="BP6">
+        <v>0</v>
+      </c>
+      <c r="BQ6">
+        <v>0</v>
+      </c>
+      <c r="BR6">
+        <v>0</v>
+      </c>
+      <c r="BS6">
+        <v>0</v>
+      </c>
+      <c r="BT6">
+        <v>0</v>
+      </c>
+      <c r="BU6">
+        <v>0</v>
+      </c>
+      <c r="BV6">
+        <v>0</v>
+      </c>
+      <c r="BW6">
+        <v>0</v>
+      </c>
+      <c r="BX6">
+        <v>0</v>
+      </c>
+      <c r="BY6">
+        <v>0</v>
+      </c>
+      <c r="BZ6">
+        <v>0</v>
+      </c>
+      <c r="CA6">
+        <v>0</v>
+      </c>
+      <c r="CB6">
+        <v>0</v>
+      </c>
+      <c r="CC6">
+        <v>0</v>
+      </c>
+      <c r="CD6">
+        <v>0</v>
+      </c>
+      <c r="CE6">
+        <v>0</v>
+      </c>
+      <c r="CF6">
+        <v>0</v>
+      </c>
+      <c r="CG6">
+        <v>0</v>
+      </c>
+      <c r="CH6">
+        <v>0</v>
+      </c>
+      <c r="CI6">
+        <v>0</v>
+      </c>
+      <c r="CJ6">
+        <v>0</v>
+      </c>
+      <c r="CK6">
+        <v>0</v>
+      </c>
+      <c r="CL6">
+        <v>0</v>
+      </c>
+      <c r="CM6">
+        <v>0</v>
+      </c>
+      <c r="CN6">
+        <v>0</v>
+      </c>
+      <c r="CO6">
+        <v>0</v>
+      </c>
+      <c r="CP6">
+        <v>0</v>
+      </c>
+      <c r="CQ6">
+        <v>0</v>
+      </c>
+      <c r="CR6">
+        <v>0</v>
+      </c>
+      <c r="CS6">
+        <v>0</v>
+      </c>
+      <c r="CT6">
+        <v>0</v>
+      </c>
+      <c r="CU6">
+        <v>0</v>
+      </c>
+      <c r="CV6">
+        <v>0</v>
+      </c>
+      <c r="CW6">
+        <v>0</v>
+      </c>
+      <c r="CX6">
+        <v>0</v>
+      </c>
+      <c r="CY6">
+        <v>0</v>
+      </c>
+      <c r="CZ6">
+        <v>0</v>
+      </c>
+      <c r="DA6">
+        <v>0</v>
+      </c>
+      <c r="DB6">
+        <v>0</v>
+      </c>
+      <c r="DC6">
+        <v>0</v>
+      </c>
+      <c r="DD6">
+        <v>0</v>
+      </c>
+      <c r="DE6">
+        <v>0</v>
+      </c>
+      <c r="DF6">
+        <v>0</v>
+      </c>
+      <c r="DG6">
+        <v>0</v>
+      </c>
+      <c r="DH6">
+        <v>0</v>
+      </c>
+      <c r="DI6">
+        <v>0</v>
+      </c>
+      <c r="DJ6">
+        <v>0</v>
+      </c>
+      <c r="DK6">
+        <v>0</v>
+      </c>
+      <c r="DL6">
+        <v>0</v>
+      </c>
+      <c r="DM6">
+        <v>0</v>
+      </c>
+      <c r="DN6">
+        <v>0</v>
+      </c>
+      <c r="DO6">
+        <v>0</v>
+      </c>
+      <c r="DP6">
+        <v>0</v>
+      </c>
+      <c r="DQ6">
+        <v>0</v>
+      </c>
+      <c r="DR6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>395</v>
       </c>
@@ -29366,8 +31412,299 @@
       <c r="Y7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
+        <v>0</v>
+      </c>
+      <c r="AX7">
+        <v>0</v>
+      </c>
+      <c r="AY7">
+        <v>0</v>
+      </c>
+      <c r="AZ7">
+        <v>0</v>
+      </c>
+      <c r="BA7">
+        <v>0</v>
+      </c>
+      <c r="BB7">
+        <v>0</v>
+      </c>
+      <c r="BC7">
+        <v>0</v>
+      </c>
+      <c r="BD7">
+        <v>0</v>
+      </c>
+      <c r="BE7">
+        <v>0</v>
+      </c>
+      <c r="BF7">
+        <v>0</v>
+      </c>
+      <c r="BG7">
+        <v>0</v>
+      </c>
+      <c r="BH7">
+        <v>0</v>
+      </c>
+      <c r="BI7">
+        <v>0</v>
+      </c>
+      <c r="BJ7">
+        <v>0</v>
+      </c>
+      <c r="BK7">
+        <v>0</v>
+      </c>
+      <c r="BL7">
+        <v>0</v>
+      </c>
+      <c r="BM7">
+        <v>0</v>
+      </c>
+      <c r="BN7">
+        <v>0</v>
+      </c>
+      <c r="BO7">
+        <v>0</v>
+      </c>
+      <c r="BP7">
+        <v>0</v>
+      </c>
+      <c r="BQ7">
+        <v>0</v>
+      </c>
+      <c r="BR7">
+        <v>0</v>
+      </c>
+      <c r="BS7">
+        <v>0</v>
+      </c>
+      <c r="BT7">
+        <v>0</v>
+      </c>
+      <c r="BU7">
+        <v>0</v>
+      </c>
+      <c r="BV7">
+        <v>0</v>
+      </c>
+      <c r="BW7">
+        <v>0</v>
+      </c>
+      <c r="BX7">
+        <v>0</v>
+      </c>
+      <c r="BY7">
+        <v>0</v>
+      </c>
+      <c r="BZ7">
+        <v>0</v>
+      </c>
+      <c r="CA7">
+        <v>0</v>
+      </c>
+      <c r="CB7">
+        <v>0</v>
+      </c>
+      <c r="CC7">
+        <v>0</v>
+      </c>
+      <c r="CD7">
+        <v>0</v>
+      </c>
+      <c r="CE7">
+        <v>0</v>
+      </c>
+      <c r="CF7">
+        <v>0</v>
+      </c>
+      <c r="CG7">
+        <v>0</v>
+      </c>
+      <c r="CH7">
+        <v>0</v>
+      </c>
+      <c r="CI7">
+        <v>0</v>
+      </c>
+      <c r="CJ7">
+        <v>0</v>
+      </c>
+      <c r="CK7">
+        <v>0</v>
+      </c>
+      <c r="CL7">
+        <v>0</v>
+      </c>
+      <c r="CM7">
+        <v>0</v>
+      </c>
+      <c r="CN7">
+        <v>0</v>
+      </c>
+      <c r="CO7">
+        <v>0</v>
+      </c>
+      <c r="CP7">
+        <v>0</v>
+      </c>
+      <c r="CQ7">
+        <v>0</v>
+      </c>
+      <c r="CR7">
+        <v>0</v>
+      </c>
+      <c r="CS7">
+        <v>0</v>
+      </c>
+      <c r="CT7">
+        <v>0</v>
+      </c>
+      <c r="CU7">
+        <v>0</v>
+      </c>
+      <c r="CV7">
+        <v>0</v>
+      </c>
+      <c r="CW7">
+        <v>0</v>
+      </c>
+      <c r="CX7">
+        <v>0</v>
+      </c>
+      <c r="CY7">
+        <v>0</v>
+      </c>
+      <c r="CZ7">
+        <v>0</v>
+      </c>
+      <c r="DA7">
+        <v>0</v>
+      </c>
+      <c r="DB7">
+        <v>0</v>
+      </c>
+      <c r="DC7">
+        <v>0</v>
+      </c>
+      <c r="DD7">
+        <v>0</v>
+      </c>
+      <c r="DE7">
+        <v>0</v>
+      </c>
+      <c r="DF7">
+        <v>0</v>
+      </c>
+      <c r="DG7">
+        <v>0</v>
+      </c>
+      <c r="DH7">
+        <v>0</v>
+      </c>
+      <c r="DI7">
+        <v>0</v>
+      </c>
+      <c r="DJ7">
+        <v>0</v>
+      </c>
+      <c r="DK7">
+        <v>0</v>
+      </c>
+      <c r="DL7">
+        <v>0</v>
+      </c>
+      <c r="DM7">
+        <v>0</v>
+      </c>
+      <c r="DN7">
+        <v>0</v>
+      </c>
+      <c r="DO7">
+        <v>0</v>
+      </c>
+      <c r="DP7">
+        <v>0</v>
+      </c>
+      <c r="DQ7">
+        <v>0</v>
+      </c>
+      <c r="DR7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>395</v>
       </c>
@@ -29443,8 +31780,299 @@
       <c r="Y8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8">
+        <v>0</v>
+      </c>
+      <c r="AX8">
+        <v>0</v>
+      </c>
+      <c r="AY8">
+        <v>0</v>
+      </c>
+      <c r="AZ8">
+        <v>0</v>
+      </c>
+      <c r="BA8">
+        <v>0</v>
+      </c>
+      <c r="BB8">
+        <v>0</v>
+      </c>
+      <c r="BC8">
+        <v>0</v>
+      </c>
+      <c r="BD8">
+        <v>0</v>
+      </c>
+      <c r="BE8">
+        <v>0</v>
+      </c>
+      <c r="BF8">
+        <v>0</v>
+      </c>
+      <c r="BG8">
+        <v>0</v>
+      </c>
+      <c r="BH8">
+        <v>0</v>
+      </c>
+      <c r="BI8">
+        <v>0</v>
+      </c>
+      <c r="BJ8">
+        <v>0</v>
+      </c>
+      <c r="BK8">
+        <v>0</v>
+      </c>
+      <c r="BL8">
+        <v>0</v>
+      </c>
+      <c r="BM8">
+        <v>0</v>
+      </c>
+      <c r="BN8">
+        <v>0</v>
+      </c>
+      <c r="BO8">
+        <v>0</v>
+      </c>
+      <c r="BP8">
+        <v>0</v>
+      </c>
+      <c r="BQ8">
+        <v>0</v>
+      </c>
+      <c r="BR8">
+        <v>0</v>
+      </c>
+      <c r="BS8">
+        <v>0</v>
+      </c>
+      <c r="BT8">
+        <v>0</v>
+      </c>
+      <c r="BU8">
+        <v>0</v>
+      </c>
+      <c r="BV8">
+        <v>0</v>
+      </c>
+      <c r="BW8">
+        <v>0</v>
+      </c>
+      <c r="BX8">
+        <v>0</v>
+      </c>
+      <c r="BY8">
+        <v>0</v>
+      </c>
+      <c r="BZ8">
+        <v>0</v>
+      </c>
+      <c r="CA8">
+        <v>0</v>
+      </c>
+      <c r="CB8">
+        <v>0</v>
+      </c>
+      <c r="CC8">
+        <v>0</v>
+      </c>
+      <c r="CD8">
+        <v>0</v>
+      </c>
+      <c r="CE8">
+        <v>0</v>
+      </c>
+      <c r="CF8">
+        <v>0</v>
+      </c>
+      <c r="CG8">
+        <v>0</v>
+      </c>
+      <c r="CH8">
+        <v>0</v>
+      </c>
+      <c r="CI8">
+        <v>0</v>
+      </c>
+      <c r="CJ8">
+        <v>0</v>
+      </c>
+      <c r="CK8">
+        <v>0</v>
+      </c>
+      <c r="CL8">
+        <v>0</v>
+      </c>
+      <c r="CM8">
+        <v>0</v>
+      </c>
+      <c r="CN8">
+        <v>0</v>
+      </c>
+      <c r="CO8">
+        <v>0</v>
+      </c>
+      <c r="CP8">
+        <v>0</v>
+      </c>
+      <c r="CQ8">
+        <v>0</v>
+      </c>
+      <c r="CR8">
+        <v>0</v>
+      </c>
+      <c r="CS8">
+        <v>0</v>
+      </c>
+      <c r="CT8">
+        <v>0</v>
+      </c>
+      <c r="CU8">
+        <v>0</v>
+      </c>
+      <c r="CV8">
+        <v>0</v>
+      </c>
+      <c r="CW8">
+        <v>0</v>
+      </c>
+      <c r="CX8">
+        <v>0</v>
+      </c>
+      <c r="CY8">
+        <v>0</v>
+      </c>
+      <c r="CZ8">
+        <v>0</v>
+      </c>
+      <c r="DA8">
+        <v>0</v>
+      </c>
+      <c r="DB8">
+        <v>0</v>
+      </c>
+      <c r="DC8">
+        <v>0</v>
+      </c>
+      <c r="DD8">
+        <v>0</v>
+      </c>
+      <c r="DE8">
+        <v>0</v>
+      </c>
+      <c r="DF8">
+        <v>0</v>
+      </c>
+      <c r="DG8">
+        <v>0</v>
+      </c>
+      <c r="DH8">
+        <v>0</v>
+      </c>
+      <c r="DI8">
+        <v>0</v>
+      </c>
+      <c r="DJ8">
+        <v>0</v>
+      </c>
+      <c r="DK8">
+        <v>0</v>
+      </c>
+      <c r="DL8">
+        <v>0</v>
+      </c>
+      <c r="DM8">
+        <v>0</v>
+      </c>
+      <c r="DN8">
+        <v>0</v>
+      </c>
+      <c r="DO8">
+        <v>0</v>
+      </c>
+      <c r="DP8">
+        <v>0</v>
+      </c>
+      <c r="DQ8">
+        <v>0</v>
+      </c>
+      <c r="DR8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>395</v>
       </c>
@@ -29520,8 +32148,299 @@
       <c r="Y9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
+      </c>
+      <c r="AV9">
+        <v>0</v>
+      </c>
+      <c r="AW9">
+        <v>0</v>
+      </c>
+      <c r="AX9">
+        <v>0</v>
+      </c>
+      <c r="AY9">
+        <v>0</v>
+      </c>
+      <c r="AZ9">
+        <v>0</v>
+      </c>
+      <c r="BA9">
+        <v>0</v>
+      </c>
+      <c r="BB9">
+        <v>0</v>
+      </c>
+      <c r="BC9">
+        <v>0</v>
+      </c>
+      <c r="BD9">
+        <v>0</v>
+      </c>
+      <c r="BE9">
+        <v>0</v>
+      </c>
+      <c r="BF9">
+        <v>0</v>
+      </c>
+      <c r="BG9">
+        <v>0</v>
+      </c>
+      <c r="BH9">
+        <v>0</v>
+      </c>
+      <c r="BI9">
+        <v>0</v>
+      </c>
+      <c r="BJ9">
+        <v>0</v>
+      </c>
+      <c r="BK9">
+        <v>0</v>
+      </c>
+      <c r="BL9">
+        <v>0</v>
+      </c>
+      <c r="BM9">
+        <v>0</v>
+      </c>
+      <c r="BN9">
+        <v>0</v>
+      </c>
+      <c r="BO9">
+        <v>0</v>
+      </c>
+      <c r="BP9">
+        <v>0</v>
+      </c>
+      <c r="BQ9">
+        <v>0</v>
+      </c>
+      <c r="BR9">
+        <v>0</v>
+      </c>
+      <c r="BS9">
+        <v>0</v>
+      </c>
+      <c r="BT9">
+        <v>0</v>
+      </c>
+      <c r="BU9">
+        <v>0</v>
+      </c>
+      <c r="BV9">
+        <v>0</v>
+      </c>
+      <c r="BW9">
+        <v>0</v>
+      </c>
+      <c r="BX9">
+        <v>0</v>
+      </c>
+      <c r="BY9">
+        <v>0</v>
+      </c>
+      <c r="BZ9">
+        <v>0</v>
+      </c>
+      <c r="CA9">
+        <v>0</v>
+      </c>
+      <c r="CB9">
+        <v>0</v>
+      </c>
+      <c r="CC9">
+        <v>0</v>
+      </c>
+      <c r="CD9">
+        <v>0</v>
+      </c>
+      <c r="CE9">
+        <v>0</v>
+      </c>
+      <c r="CF9">
+        <v>0</v>
+      </c>
+      <c r="CG9">
+        <v>0</v>
+      </c>
+      <c r="CH9">
+        <v>0</v>
+      </c>
+      <c r="CI9">
+        <v>0</v>
+      </c>
+      <c r="CJ9">
+        <v>0</v>
+      </c>
+      <c r="CK9">
+        <v>0</v>
+      </c>
+      <c r="CL9">
+        <v>0</v>
+      </c>
+      <c r="CM9">
+        <v>0</v>
+      </c>
+      <c r="CN9">
+        <v>0</v>
+      </c>
+      <c r="CO9">
+        <v>0</v>
+      </c>
+      <c r="CP9">
+        <v>0</v>
+      </c>
+      <c r="CQ9">
+        <v>0</v>
+      </c>
+      <c r="CR9">
+        <v>0</v>
+      </c>
+      <c r="CS9">
+        <v>0</v>
+      </c>
+      <c r="CT9">
+        <v>0</v>
+      </c>
+      <c r="CU9">
+        <v>0</v>
+      </c>
+      <c r="CV9">
+        <v>0</v>
+      </c>
+      <c r="CW9">
+        <v>0</v>
+      </c>
+      <c r="CX9">
+        <v>0</v>
+      </c>
+      <c r="CY9">
+        <v>0</v>
+      </c>
+      <c r="CZ9">
+        <v>0</v>
+      </c>
+      <c r="DA9">
+        <v>0</v>
+      </c>
+      <c r="DB9">
+        <v>0</v>
+      </c>
+      <c r="DC9">
+        <v>0</v>
+      </c>
+      <c r="DD9">
+        <v>0</v>
+      </c>
+      <c r="DE9">
+        <v>0</v>
+      </c>
+      <c r="DF9">
+        <v>0</v>
+      </c>
+      <c r="DG9">
+        <v>0</v>
+      </c>
+      <c r="DH9">
+        <v>0</v>
+      </c>
+      <c r="DI9">
+        <v>0</v>
+      </c>
+      <c r="DJ9">
+        <v>0</v>
+      </c>
+      <c r="DK9">
+        <v>0</v>
+      </c>
+      <c r="DL9">
+        <v>0</v>
+      </c>
+      <c r="DM9">
+        <v>0</v>
+      </c>
+      <c r="DN9">
+        <v>0</v>
+      </c>
+      <c r="DO9">
+        <v>0</v>
+      </c>
+      <c r="DP9">
+        <v>0</v>
+      </c>
+      <c r="DQ9">
+        <v>0</v>
+      </c>
+      <c r="DR9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>395</v>
       </c>
@@ -29597,8 +32516,299 @@
       <c r="Y10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>0</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+      <c r="AT10">
+        <v>0</v>
+      </c>
+      <c r="AU10">
+        <v>0</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10">
+        <v>0</v>
+      </c>
+      <c r="AX10">
+        <v>0</v>
+      </c>
+      <c r="AY10">
+        <v>0</v>
+      </c>
+      <c r="AZ10">
+        <v>0</v>
+      </c>
+      <c r="BA10">
+        <v>0</v>
+      </c>
+      <c r="BB10">
+        <v>0</v>
+      </c>
+      <c r="BC10">
+        <v>0</v>
+      </c>
+      <c r="BD10">
+        <v>0</v>
+      </c>
+      <c r="BE10">
+        <v>0</v>
+      </c>
+      <c r="BF10">
+        <v>0</v>
+      </c>
+      <c r="BG10">
+        <v>0</v>
+      </c>
+      <c r="BH10">
+        <v>0</v>
+      </c>
+      <c r="BI10">
+        <v>0</v>
+      </c>
+      <c r="BJ10">
+        <v>0</v>
+      </c>
+      <c r="BK10">
+        <v>0</v>
+      </c>
+      <c r="BL10">
+        <v>0</v>
+      </c>
+      <c r="BM10">
+        <v>0</v>
+      </c>
+      <c r="BN10">
+        <v>0</v>
+      </c>
+      <c r="BO10">
+        <v>0</v>
+      </c>
+      <c r="BP10">
+        <v>0</v>
+      </c>
+      <c r="BQ10">
+        <v>0</v>
+      </c>
+      <c r="BR10">
+        <v>0</v>
+      </c>
+      <c r="BS10">
+        <v>0</v>
+      </c>
+      <c r="BT10">
+        <v>0</v>
+      </c>
+      <c r="BU10">
+        <v>0</v>
+      </c>
+      <c r="BV10">
+        <v>0</v>
+      </c>
+      <c r="BW10">
+        <v>0</v>
+      </c>
+      <c r="BX10">
+        <v>0</v>
+      </c>
+      <c r="BY10">
+        <v>0</v>
+      </c>
+      <c r="BZ10">
+        <v>0</v>
+      </c>
+      <c r="CA10">
+        <v>0</v>
+      </c>
+      <c r="CB10">
+        <v>0</v>
+      </c>
+      <c r="CC10">
+        <v>0</v>
+      </c>
+      <c r="CD10">
+        <v>0</v>
+      </c>
+      <c r="CE10">
+        <v>0</v>
+      </c>
+      <c r="CF10">
+        <v>0</v>
+      </c>
+      <c r="CG10">
+        <v>0</v>
+      </c>
+      <c r="CH10">
+        <v>0</v>
+      </c>
+      <c r="CI10">
+        <v>0</v>
+      </c>
+      <c r="CJ10">
+        <v>0</v>
+      </c>
+      <c r="CK10">
+        <v>0</v>
+      </c>
+      <c r="CL10">
+        <v>0</v>
+      </c>
+      <c r="CM10">
+        <v>0</v>
+      </c>
+      <c r="CN10">
+        <v>0</v>
+      </c>
+      <c r="CO10">
+        <v>0</v>
+      </c>
+      <c r="CP10">
+        <v>0</v>
+      </c>
+      <c r="CQ10">
+        <v>0</v>
+      </c>
+      <c r="CR10">
+        <v>0</v>
+      </c>
+      <c r="CS10">
+        <v>0</v>
+      </c>
+      <c r="CT10">
+        <v>0</v>
+      </c>
+      <c r="CU10">
+        <v>0</v>
+      </c>
+      <c r="CV10">
+        <v>0</v>
+      </c>
+      <c r="CW10">
+        <v>0</v>
+      </c>
+      <c r="CX10">
+        <v>0</v>
+      </c>
+      <c r="CY10">
+        <v>0</v>
+      </c>
+      <c r="CZ10">
+        <v>0</v>
+      </c>
+      <c r="DA10">
+        <v>0</v>
+      </c>
+      <c r="DB10">
+        <v>0</v>
+      </c>
+      <c r="DC10">
+        <v>0</v>
+      </c>
+      <c r="DD10">
+        <v>0</v>
+      </c>
+      <c r="DE10">
+        <v>0</v>
+      </c>
+      <c r="DF10">
+        <v>0</v>
+      </c>
+      <c r="DG10">
+        <v>0</v>
+      </c>
+      <c r="DH10">
+        <v>0</v>
+      </c>
+      <c r="DI10">
+        <v>0</v>
+      </c>
+      <c r="DJ10">
+        <v>0</v>
+      </c>
+      <c r="DK10">
+        <v>0</v>
+      </c>
+      <c r="DL10">
+        <v>0</v>
+      </c>
+      <c r="DM10">
+        <v>0</v>
+      </c>
+      <c r="DN10">
+        <v>0</v>
+      </c>
+      <c r="DO10">
+        <v>0</v>
+      </c>
+      <c r="DP10">
+        <v>0</v>
+      </c>
+      <c r="DQ10">
+        <v>0</v>
+      </c>
+      <c r="DR10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>395</v>
       </c>
@@ -29674,8 +32884,299 @@
       <c r="Y11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+      <c r="AS11">
+        <v>0</v>
+      </c>
+      <c r="AT11">
+        <v>0</v>
+      </c>
+      <c r="AU11">
+        <v>0</v>
+      </c>
+      <c r="AV11">
+        <v>0</v>
+      </c>
+      <c r="AW11">
+        <v>0</v>
+      </c>
+      <c r="AX11">
+        <v>0</v>
+      </c>
+      <c r="AY11">
+        <v>0</v>
+      </c>
+      <c r="AZ11">
+        <v>0</v>
+      </c>
+      <c r="BA11">
+        <v>0</v>
+      </c>
+      <c r="BB11">
+        <v>0</v>
+      </c>
+      <c r="BC11">
+        <v>0</v>
+      </c>
+      <c r="BD11">
+        <v>0</v>
+      </c>
+      <c r="BE11">
+        <v>0</v>
+      </c>
+      <c r="BF11">
+        <v>0</v>
+      </c>
+      <c r="BG11">
+        <v>0</v>
+      </c>
+      <c r="BH11">
+        <v>0</v>
+      </c>
+      <c r="BI11">
+        <v>0</v>
+      </c>
+      <c r="BJ11">
+        <v>0</v>
+      </c>
+      <c r="BK11">
+        <v>0</v>
+      </c>
+      <c r="BL11">
+        <v>0</v>
+      </c>
+      <c r="BM11">
+        <v>0</v>
+      </c>
+      <c r="BN11">
+        <v>0</v>
+      </c>
+      <c r="BO11">
+        <v>0</v>
+      </c>
+      <c r="BP11">
+        <v>0</v>
+      </c>
+      <c r="BQ11">
+        <v>0</v>
+      </c>
+      <c r="BR11">
+        <v>0</v>
+      </c>
+      <c r="BS11">
+        <v>0</v>
+      </c>
+      <c r="BT11">
+        <v>0</v>
+      </c>
+      <c r="BU11">
+        <v>0</v>
+      </c>
+      <c r="BV11">
+        <v>0</v>
+      </c>
+      <c r="BW11">
+        <v>0</v>
+      </c>
+      <c r="BX11">
+        <v>0</v>
+      </c>
+      <c r="BY11">
+        <v>0</v>
+      </c>
+      <c r="BZ11">
+        <v>0</v>
+      </c>
+      <c r="CA11">
+        <v>0</v>
+      </c>
+      <c r="CB11">
+        <v>0</v>
+      </c>
+      <c r="CC11">
+        <v>0</v>
+      </c>
+      <c r="CD11">
+        <v>0</v>
+      </c>
+      <c r="CE11">
+        <v>0</v>
+      </c>
+      <c r="CF11">
+        <v>0</v>
+      </c>
+      <c r="CG11">
+        <v>0</v>
+      </c>
+      <c r="CH11">
+        <v>0</v>
+      </c>
+      <c r="CI11">
+        <v>0</v>
+      </c>
+      <c r="CJ11">
+        <v>0</v>
+      </c>
+      <c r="CK11">
+        <v>0</v>
+      </c>
+      <c r="CL11">
+        <v>0</v>
+      </c>
+      <c r="CM11">
+        <v>0</v>
+      </c>
+      <c r="CN11">
+        <v>0</v>
+      </c>
+      <c r="CO11">
+        <v>0</v>
+      </c>
+      <c r="CP11">
+        <v>0</v>
+      </c>
+      <c r="CQ11">
+        <v>0</v>
+      </c>
+      <c r="CR11">
+        <v>0</v>
+      </c>
+      <c r="CS11">
+        <v>0</v>
+      </c>
+      <c r="CT11">
+        <v>0</v>
+      </c>
+      <c r="CU11">
+        <v>0</v>
+      </c>
+      <c r="CV11">
+        <v>0</v>
+      </c>
+      <c r="CW11">
+        <v>0</v>
+      </c>
+      <c r="CX11">
+        <v>0</v>
+      </c>
+      <c r="CY11">
+        <v>0</v>
+      </c>
+      <c r="CZ11">
+        <v>0</v>
+      </c>
+      <c r="DA11">
+        <v>0</v>
+      </c>
+      <c r="DB11">
+        <v>0</v>
+      </c>
+      <c r="DC11">
+        <v>0</v>
+      </c>
+      <c r="DD11">
+        <v>0</v>
+      </c>
+      <c r="DE11">
+        <v>0</v>
+      </c>
+      <c r="DF11">
+        <v>0</v>
+      </c>
+      <c r="DG11">
+        <v>0</v>
+      </c>
+      <c r="DH11">
+        <v>0</v>
+      </c>
+      <c r="DI11">
+        <v>0</v>
+      </c>
+      <c r="DJ11">
+        <v>0</v>
+      </c>
+      <c r="DK11">
+        <v>0</v>
+      </c>
+      <c r="DL11">
+        <v>0</v>
+      </c>
+      <c r="DM11">
+        <v>0</v>
+      </c>
+      <c r="DN11">
+        <v>0</v>
+      </c>
+      <c r="DO11">
+        <v>0</v>
+      </c>
+      <c r="DP11">
+        <v>0</v>
+      </c>
+      <c r="DQ11">
+        <v>0</v>
+      </c>
+      <c r="DR11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>395</v>
       </c>
@@ -29751,8 +33252,26 @@
       <c r="Y12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>395</v>
       </c>
@@ -29828,8 +33347,26 @@
       <c r="Y13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>395</v>
       </c>
@@ -29905,8 +33442,26 @@
       <c r="Y14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>395</v>
       </c>
@@ -29982,8 +33537,26 @@
       <c r="Y15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>395</v>
       </c>
@@ -30059,8 +33632,26 @@
       <c r="Y16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>395</v>
       </c>
@@ -30136,8 +33727,26 @@
       <c r="Y17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>395</v>
       </c>
@@ -30213,8 +33822,26 @@
       <c r="Y18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>395</v>
       </c>
@@ -30290,8 +33917,26 @@
       <c r="Y19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>395</v>
       </c>
@@ -30367,8 +34012,26 @@
       <c r="Y20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>395</v>
       </c>
@@ -30442,6 +34105,24 @@
         <v>0</v>
       </c>
       <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New script for updating SS outputs for CEATTLE
</commit_message>
<xml_diff>
--- a/data/hake_from_ss.xlsx
+++ b/data/hake_from_ss.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1207EA80-0E56-7B40-B2F3-7AB71055A8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5925D8C3-E0E8-EE4B-B074-847C390C95AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="42700" firstSheet="3" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="493">
   <si>
     <t>Number</t>
   </si>
@@ -8957,15 +8957,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -9029,8 +9029,38 @@
       <c r="U1" s="1" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9286,7 +9316,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9353,7 +9383,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9425,7 +9455,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9446,10 +9476,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>5.5313539999999996E-3</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>3.0459800000000001</v>
       </c>
     </row>
   </sheetData>
@@ -9580,7 +9610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -13873,8 +13903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13973,7 +14003,7 @@
         <v>49</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -28645,7 +28675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>

</xml_diff>